<commit_message>
add changes in xlsx; add SQL-table.db
</commit_message>
<xml_diff>
--- a/Excel-Table/SQL_table.xlsx
+++ b/Excel-Table/SQL_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="abbreviation" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="category_assignment" sheetId="3" r:id="rId3"/>
     <sheet name="parent_children" sheetId="4" r:id="rId4"/>
     <sheet name="Tabellen für Excel" sheetId="5" r:id="rId5"/>
+    <sheet name="BUDO Key" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="category_name_german">category[category_name_german]</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="216">
   <si>
     <t>Betonkerntemperierung</t>
   </si>
@@ -211,9 +212,6 @@
     <t>Kältespeicher</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Kombispeicher</t>
   </si>
   <si>
@@ -223,9 +221,6 @@
     <t>Wärmespeicher</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>Warmwasser (TW)</t>
   </si>
   <si>
@@ -662,13 +657,37 @@
   </si>
   <si>
     <t>Kürzel</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>C.STO</t>
+  </si>
+  <si>
+    <t>H.STO</t>
+  </si>
+  <si>
+    <t>INTEGER[10]</t>
+  </si>
+  <si>
+    <t>VARCHAR[1000]</t>
+  </si>
+  <si>
+    <t>VARCHAR[30]</t>
+  </si>
+  <si>
+    <t>abbreviation_BUDO</t>
+  </si>
+  <si>
+    <t>VARCHAR[200]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +716,13 @@
     <font>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -741,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -753,32 +779,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -848,6 +855,27 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -895,13 +923,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="abbreviation" displayName="abbreviation" ref="A1:E41" totalsRowShown="0">
-  <autoFilter ref="A1:E41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="abbreviation" displayName="abbreviation" ref="A2:E42" totalsRowShown="0">
+  <autoFilter ref="A2:E42"/>
   <tableColumns count="5">
     <tableColumn id="1" name="abbreviation_id"/>
     <tableColumn id="2" name="description_german" dataDxfId="17"/>
     <tableColumn id="4" name="description_english" dataDxfId="16"/>
-    <tableColumn id="3" name="abbreviation"/>
+    <tableColumn id="3" name="abbreviation_BUDO"/>
     <tableColumn id="5" name="abbreviation_id(for SVERWEIS)" dataDxfId="15">
       <calculatedColumnFormula>abbreviation[[#This Row],[abbreviation_id]]</calculatedColumnFormula>
     </tableColumn>
@@ -911,15 +939,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="category" displayName="category" ref="A1:F41" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:F41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="category" displayName="category" ref="A2:F42" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F42"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="category_id" dataDxfId="12"/>
-    <tableColumn id="2" name="category_name_german" dataDxfId="11"/>
-    <tableColumn id="3" name="category_name_english" dataDxfId="10"/>
-    <tableColumn id="4" name="abbreviation" dataDxfId="9"/>
-    <tableColumn id="5" name="comment" dataDxfId="8"/>
-    <tableColumn id="6" name="category_id(for SVERWEIS)" dataDxfId="7">
+    <tableColumn id="1" name="category_id" dataDxfId="5"/>
+    <tableColumn id="2" name="category_name_german" dataDxfId="4"/>
+    <tableColumn id="3" name="category_name_english" dataDxfId="3"/>
+    <tableColumn id="4" name="abbreviation" dataDxfId="2"/>
+    <tableColumn id="5" name="comment" dataDxfId="1"/>
+    <tableColumn id="6" name="category_id(for SVERWEIS)" dataDxfId="0">
       <calculatedColumnFormula>category[[#This Row],[category_id]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -940,16 +968,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle8" displayName="Tabelle8" ref="E1:G25" totalsRowShown="0">
-  <autoFilter ref="E1:G25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle8" displayName="Tabelle8" ref="E1:G35" totalsRowShown="0">
+  <autoFilter ref="E1:G35"/>
   <tableColumns count="3">
     <tableColumn id="1" name="category_assignment_id">
       <calculatedColumnFormula>category_assignment[[#This Row],[category_assignment_id]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="category_id" dataDxfId="6">
+    <tableColumn id="2" name="category_id" dataDxfId="14">
       <calculatedColumnFormula>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="abbreviation_id" dataDxfId="5">
+    <tableColumn id="3" name="abbreviation_id" dataDxfId="13">
       <calculatedColumnFormula>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -973,13 +1001,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="parent_children8" displayName="parent_children8" ref="E1:G25" totalsRowShown="0">
   <autoFilter ref="E1:G25"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="parent_children_id" dataDxfId="4">
+    <tableColumn id="1" name="parent_children_id" dataDxfId="12">
       <calculatedColumnFormula>parent_children[[#This Row],[parent_children_id]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="parent_id" dataDxfId="3">
+    <tableColumn id="2" name="parent_id" dataDxfId="11">
       <calculatedColumnFormula>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="children_id" dataDxfId="2">
+    <tableColumn id="3" name="children_id" dataDxfId="10">
       <calculatedColumnFormula>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -993,10 +1021,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="System"/>
     <tableColumn id="2" name="."/>
-    <tableColumn id="3" name="System_2" dataDxfId="1">
-      <calculatedColumnFormula>IF(I2="","", VLOOKUP(I2, parent_children[[parent]:[children]], 2,'FALSE'))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" name="System_3" dataDxfId="0">
+    <tableColumn id="3" name="System_2" dataDxfId="9"/>
+    <tableColumn id="4" name="System_3" dataDxfId="8">
       <calculatedColumnFormula>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1267,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1278,689 +1304,863 @@
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="0.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="6" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
         <v>194</v>
       </c>
-      <c r="B1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="6" customFormat="1">
-      <c r="A2" s="6">
+      <c r="C2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G2" t="str">
+        <f ca="1">"CREATE TABLE "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;"("&amp;abbreviation[[#Headers],[abbreviation_id]]&amp;" "&amp;A1&amp;","&amp;abbreviation[[#Headers],[description_german]]&amp;" "&amp;B1&amp;","&amp;abbreviation[[#Headers],[description_english]]&amp;" "&amp;C1&amp;","&amp;abbreviation[[#Headers],[abbreviation_BUDO]]&amp;" "&amp;D1&amp;", PRIMARY KEY("&amp;abbreviation[[#Headers],[abbreviation_id]]&amp;"))"</f>
+        <v>CREATE TABLE abbreviation(abbreviation_id INTEGER[10],description_german VARCHAR[1000],description_english VARCHAR[1000],abbreviation_BUDO VARCHAR[30], PRIMARY KEY(abbreviation_id))</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1">
+      <c r="A3" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="E2" s="6">
+      <c r="B3" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="E3" s="6">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
+      <c r="G3" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (0,' ,,);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
+      <c r="G4" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (1,Betonkerntemperierung,,CCA);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
+      <c r="G5" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (2,Blockheizkraftwerk (BHKW),,CHP);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
+      <c r="G6" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (3,Fernkälte,,C.DISCT);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
+      <c r="G7" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (4,Fernwärme,,H.DISCT);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
+      <c r="G8" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (5,Freie Kühlung,,C.FREE);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
+      <c r="G9" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (6,Gaskühler,,C.GAS);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
+      <c r="G10" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (7,Gebäudeautomationssystem,,BAS);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
+      <c r="G11" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (8,Gebäudemanagementsystem,,BMS);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
+      <c r="G12" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (9,Kältemaschine,,CH);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
+      <c r="G13" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (10,Kessel,,BOI);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
         <v>11</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
+      <c r="G14" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (11,Kühlturm,,C.TOW);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
+      <c r="G15" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (12,Luft,,AIR);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
         <v>13</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="G16" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (13,Lüftungsmaschine,,AHU);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
+      <c r="G17" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (14,Solarthermie,,SOL.TH);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
         <v>15</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
+      <c r="G18" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (15,Speicher,,STO);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
         <v>16</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
+      <c r="G19" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (16,Unterverteiler,,DIST.SUB);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
+      <c r="G20" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (17,Unterverteilsystem,,DISTS.SUB);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
         <v>18</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
+      <c r="G21" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (18,Verteiler,,DIST);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
         <v>19</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7" t="s">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
+      <c r="G22" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (19,Verteilsystem,,DISTS);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
         <v>20</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
+      <c r="G23" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (20,Wärmepumpe,,HP);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
+      <c r="G24" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (21,Wärmeübertrager,,HX);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
         <v>22</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
+      <c r="G25" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (22,Wasser,,WS);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
         <v>23</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
+      <c r="G26" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (23,Rückkühlung,,RCOO);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7" t="s">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27">
+      <c r="G27" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (24,Geothermiefeld,,GTF);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
         <v>25</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7" t="s">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28">
+      <c r="G28" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (25,Brennwertkessel,,COND);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
         <v>26</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7" t="s">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
+      <c r="G29" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (26,Festbrennstoffkessel,,SFUEL);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
         <v>27</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7" t="s">
+      <c r="C30" s="7"/>
+      <c r="D30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
+      <c r="G30" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (27,Niedertemperaturkessel,,LT);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
         <v>28</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B31" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="7" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31">
+      <c r="G31" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (28,Absorption,,ABSPT);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
         <v>29</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7" t="s">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32">
+      <c r="G32" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (29,Kompression,,COMP);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
         <v>30</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32">
+      <c r="C33" s="7"/>
+      <c r="D33" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="E33">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33">
+      <c r="G33" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (30,Kältespeicher,,C.STO);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
         <v>31</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B34" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33">
+      <c r="E34">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34">
+      <c r="G34" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (31,Kombispeicher,,HDH);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
         <v>32</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34">
+      <c r="B35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="E35">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35">
+      <c r="G35" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (32,Wärmespeicher,,H.STO);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
         <v>33</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35">
+      <c r="B36" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36">
+      <c r="G36" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (33,Warmwasser (TW),,DH);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
         <v>34</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36">
+      <c r="B37" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37">
+      <c r="G37" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (34,Hochtemperatur,,HT);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
         <v>35</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7" t="s">
+      <c r="B38" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E37">
+      <c r="E38">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38">
+      <c r="G38" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (35,Kälte,,CH);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="5" t="s">
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39">
+      <c r="G39" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (36,Niedertemperatur,,LT);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E39">
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40">
+      <c r="G40" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (37,Verdampfer,,EVAP);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="5" t="s">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41">
+      <c r="G41" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (38,Verdichter,,COMP);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="5" t="s">
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="G42" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (39,Verflüssiger,,COND);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:7">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:7">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:7">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:7">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:7">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
@@ -1984,20 +2184,25 @@
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
     </row>
+    <row r="54" spans="2:3">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2007,828 +2212,1004 @@
     <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="0.42578125" customWidth="1"/>
+    <col min="6" max="6" width="0.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="6" customFormat="1">
-      <c r="A2" s="7">
+    <row r="1" spans="1:8" s="6" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" t="str">
+        <f ca="1">"CREATE TABLE "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;"("&amp;category[[#Headers],[category_id]]&amp;" "&amp;A1&amp;","&amp;category[[#Headers],[category_name_german]]&amp;" "&amp;B1&amp;","&amp;category[[#Headers],[category_name_english]]&amp;" "&amp;C1&amp;","&amp;category[[#Headers],[abbreviation]]&amp;" "&amp;D1&amp;","&amp;category[[#Headers],[comment]]&amp;" "&amp;E1&amp;", PRIMARY KEY("&amp;category[[#Headers],[category_id]]&amp;"))"</f>
+        <v>CREATE TABLE abbreviation(category_id INTEGER[10],category_name_german VARCHAR[200],category_name_english VARCHAR[200],abbreviation VARCHAR[30],comment VARCHAR[1000], PRIMARY KEY(category_id))</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="6" customFormat="1">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="7">
+      <c r="H3" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;","&amp;category[[#This Row],[category_name_german]]&amp;","&amp;category[[#This Row],[category_name_english]]&amp;","&amp;category[[#This Row],[abbreviation]]&amp;","&amp;category[[#This Row],[comment]]&amp;");"</f>
+        <v>INSERT INTO abbreviation (0,,,,);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F3" s="7">
+      <c r="B4" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7">
+      <c r="H4" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (1,'System','System','SYS','not used as abbrevation');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="B5" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F5" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="7">
+      <c r="H5" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (2,'Subsystem','Subsystem','SSYS','not used as abbrevation');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="B6" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="7">
+      <c r="H6" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (3,'Subsubsystem','Subsubsystem','SSSYS','not used as abbrevation');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="B7" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F7" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7">
+      <c r="H7" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (4,'Medium','Medium','MED','not used as abbrevation');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="B8" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F7" s="7">
+      <c r="D8" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F8" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="7">
+      <c r="H8" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (5,'Position Anlage','Position device','POSA','not used as abbrevation');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="B9" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="7">
+      <c r="H9" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (6,'Datenpunkt','Data Point','DP','not used as abbrevation');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="B10" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F9" s="7">
+      <c r="F10" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="7">
+      <c r="H10" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (7,'Funktionsart','Function type','FT','not used as abbrevation');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7">
-        <f>category[[#This Row],[category_id]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="7">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>8</v>
+      </c>
+      <c r="H11" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (8,'Gebäude','building','BL','');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="7">
-        <v>10</v>
-      </c>
       <c r="B12" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>9</v>
+      </c>
+      <c r="H12" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (9,'Liegenschaft/Standort/Werk','location','L','');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="7">
-        <v>11</v>
-      </c>
       <c r="B13" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>10</v>
+      </c>
+      <c r="H13" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (10,'Gewerk','craft','CR','');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="7">
-        <v>12</v>
-      </c>
       <c r="B14" s="7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>11</v>
+      </c>
+      <c r="H14" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (11,'Raum Gerät','room device','R.D','');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="7">
-        <v>13</v>
-      </c>
       <c r="B15" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>12</v>
+      </c>
+      <c r="H15" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (12,'Geschoss Gerät','floor device','FL.D','');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="7">
-        <v>14</v>
-      </c>
       <c r="B16" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>13</v>
+      </c>
+      <c r="H16" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (13,'Gebäudeteil Gerät','section device','SC.D','');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="7">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="7">
-        <v>15</v>
-      </c>
       <c r="B17" s="7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>14</v>
+      </c>
+      <c r="H17" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (14,'Zone','zone','Z','');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="7">
-        <v>16</v>
-      </c>
       <c r="B18" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>15</v>
+      </c>
+      <c r="H18" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (15,'Fertigungsinsel/Fertigungslinie','production line','PL','');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="7">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="7">
-        <v>17</v>
-      </c>
       <c r="B19" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>16</v>
+      </c>
+      <c r="H19" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (16,'Informationsschwerpunkt','information focus','ISP','');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="7">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="7">
-        <v>18</v>
-      </c>
       <c r="B20" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7">
         <f>category[[#This Row],[category_id]]</f>
+        <v>17</v>
+      </c>
+      <c r="H20" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (17,'Wirtschaftseinheit/Kostengruppe','accounting entity','AE','');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="7">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="7">
+      <c r="B21" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7">
+        <f>category[[#This Row],[category_id]]</f>
+        <v>18</v>
+      </c>
+      <c r="H21" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (18,'Land','country','CTRY','');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="7">
         <v>19</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8">
-        <f>category[[#This Row],[category_id]]</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="7">
-        <v>20</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>19</v>
+      </c>
+      <c r="H22" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (19,'Typ der Netzwerkanbindung','network protocol','NP','');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="7">
-        <v>21</v>
-      </c>
       <c r="B23" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>20</v>
+      </c>
+      <c r="H23" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (20,'Netzwerknummer','network number','NET.N','');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="7">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="7">
-        <v>22</v>
-      </c>
       <c r="B24" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>21</v>
+      </c>
+      <c r="H24" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (21,'Raum Schaltschrank','room control cabinet','R.CC','');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="7">
-        <v>23</v>
-      </c>
       <c r="B25" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>22</v>
+      </c>
+      <c r="H25" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (22,'Geschoss Schaltschrank','floor control cabinet','FL.CC','');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="7">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="7">
-        <v>24</v>
-      </c>
       <c r="B26" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>23</v>
+      </c>
+      <c r="H26" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (23,'Gebäudeteil Schaltschrank','section control cabinet','SC.CC','');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="7">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="7">
-        <v>25</v>
-      </c>
       <c r="B27" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>24</v>
+      </c>
+      <c r="H27" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (24,'Dokumentenart/Planart','document type','DT','');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="7">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="7">
-        <v>26</v>
-      </c>
       <c r="B28" s="7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>25</v>
+      </c>
+      <c r="H28" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (25,'Unternehmen','company','CMPY','');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="7">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="7">
-        <v>27</v>
-      </c>
       <c r="B29" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>26</v>
+      </c>
+      <c r="H29" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (26,'Fabrikat/Hersteller','manufacturer','MAN','');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="7">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="7">
-        <v>28</v>
-      </c>
       <c r="B30" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>27</v>
+      </c>
+      <c r="H30" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (27,'Servername','server name','SN','');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="7">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="7">
-        <v>29</v>
-      </c>
       <c r="B31" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>28</v>
+      </c>
+      <c r="H31" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (28,'Steuerungsgruppe','control group','CG','');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="7">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="7">
-        <v>30</v>
-      </c>
       <c r="B32" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>29</v>
+      </c>
+      <c r="H32" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (29,'Größe','size','SZ','');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="7">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="7">
-        <v>31</v>
-      </c>
       <c r="B33" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>30</v>
+      </c>
+      <c r="H33" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (30,'Zählernummer','counter number','CN.N','');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="7">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="7">
-        <v>32</v>
-      </c>
       <c r="B34" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>31</v>
+      </c>
+      <c r="H34" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (31,'Achse','axis','AX','');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="7">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="7">
-        <v>33</v>
-      </c>
       <c r="B35" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>32</v>
+      </c>
+      <c r="H35" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (32,'Straße','street','STR','');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="7">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="7">
-        <v>34</v>
-      </c>
       <c r="B36" s="7" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>33</v>
+      </c>
+      <c r="H36" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (33,'Hausnummer','street number','STR.N','');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="7">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="7">
-        <v>35</v>
-      </c>
       <c r="B37" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>34</v>
+      </c>
+      <c r="H37" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (34,'Einheit','unit','U','');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="7">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="7">
-        <v>36</v>
-      </c>
       <c r="B38" s="7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>35</v>
+      </c>
+      <c r="H38" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (35,'Versorgter Raum','supplied room','R.SUP','');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="7">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="7">
-        <v>37</v>
-      </c>
       <c r="B39" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>36</v>
+      </c>
+      <c r="H39" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (36,'Versorgtes Geschoss','supplied floor','FL.SUP','');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="7">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="7">
-        <v>38</v>
-      </c>
       <c r="B40" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>37</v>
+      </c>
+      <c r="H40" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (37,'Versorgte Zone','supplied zone','Z.SUP','');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="7">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="7">
-        <v>39</v>
-      </c>
       <c r="B41" s="7" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="8">
         <f>category[[#This Row],[category_id]]</f>
+        <v>38</v>
+      </c>
+      <c r="H41" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (38,'Versorgter Gebäudeteil','supplied section','SC.SUP','');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="7">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="C42" s="7"/>
+      <c r="B42" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="F42" s="8">
+        <f>category[[#This Row],[category_id]]</f>
+        <v>39</v>
+      </c>
+      <c r="H42" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation (39,'Versorgtes Gebäude','supplied building','BL.SUP','');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="C43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:8">
       <c r="C44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:8">
       <c r="C45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:8">
       <c r="C46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:8">
       <c r="C47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:8">
       <c r="C48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="8"/>
@@ -2852,6 +3233,11 @@
       <c r="C52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="3:6">
+      <c r="C53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2866,7 +3252,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I25"/>
+      <selection activeCell="G9" sqref="A6:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2883,22 +3269,22 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
         <v>193</v>
       </c>
-      <c r="B1" t="s">
-        <v>195</v>
-      </c>
       <c r="C1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2906,7 +3292,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2929,7 +3315,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -2953,7 +3339,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -2977,7 +3363,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -3001,7 +3387,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -3025,7 +3411,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
@@ -3049,7 +3435,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -3073,7 +3459,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -3097,7 +3483,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>16</v>
@@ -3121,7 +3507,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
@@ -3145,7 +3531,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
@@ -3169,7 +3555,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>22</v>
@@ -3193,7 +3579,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>24</v>
@@ -3217,7 +3603,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>26</v>
@@ -3241,7 +3627,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -3265,7 +3651,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>30</v>
@@ -3289,7 +3675,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -3313,7 +3699,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>34</v>
@@ -3337,7 +3723,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>36</v>
@@ -3361,7 +3747,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>38</v>
@@ -3385,7 +3771,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>40</v>
@@ -3409,7 +3795,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>42</v>
@@ -3433,7 +3819,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>44</v>
@@ -3457,7 +3843,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>46</v>
@@ -3481,7 +3867,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>174</v>
+        <v>172</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>25</v>
+      </c>
+      <c r="F26" s="11">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="G26" s="11">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>2</v>
       </c>
       <c r="I26" s="6" t="str">
         <f t="array" ref="I26">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I25))),"")</f>
@@ -3492,6 +3893,18 @@
       <c r="A27" s="6">
         <v>26</v>
       </c>
+      <c r="E27">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>26</v>
+      </c>
+      <c r="F27" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G27" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I27" s="6" t="str">
         <f t="array" ref="I27">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I26))),"")</f>
         <v/>
@@ -3501,6 +3914,18 @@
       <c r="A28" s="6">
         <v>27</v>
       </c>
+      <c r="E28">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>27</v>
+      </c>
+      <c r="F28" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G28" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I28" s="6" t="str">
         <f t="array" ref="I28">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I27))),"")</f>
         <v/>
@@ -3510,6 +3935,18 @@
       <c r="A29" s="6">
         <v>28</v>
       </c>
+      <c r="E29">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>28</v>
+      </c>
+      <c r="F29" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G29" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I29" s="6" t="str">
         <f t="array" ref="I29">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I28))),"")</f>
         <v/>
@@ -3519,6 +3956,18 @@
       <c r="A30" s="6">
         <v>29</v>
       </c>
+      <c r="E30">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>29</v>
+      </c>
+      <c r="F30" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G30" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I30" s="6" t="str">
         <f t="array" ref="I30">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I29))),"")</f>
         <v/>
@@ -3528,6 +3977,18 @@
       <c r="A31" s="6">
         <v>30</v>
       </c>
+      <c r="E31">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>30</v>
+      </c>
+      <c r="F31" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G31" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I31" s="6" t="str">
         <f t="array" ref="I31">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I30))),"")</f>
         <v/>
@@ -3537,6 +3998,18 @@
       <c r="A32" s="6">
         <v>31</v>
       </c>
+      <c r="E32">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>31</v>
+      </c>
+      <c r="F32" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G32" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I32" s="6" t="str">
         <f t="array" ref="I32">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I31))),"")</f>
         <v/>
@@ -3546,6 +4019,18 @@
       <c r="A33" s="6">
         <v>32</v>
       </c>
+      <c r="E33">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>32</v>
+      </c>
+      <c r="F33" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G33" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I33" s="6" t="str">
         <f t="array" ref="I33">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I32))),"")</f>
         <v/>
@@ -3555,10 +4040,34 @@
       <c r="A34" s="6">
         <v>33</v>
       </c>
+      <c r="E34">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>33</v>
+      </c>
+      <c r="F34" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G34" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="6">
         <v>34</v>
+      </c>
+      <c r="E35">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>34</v>
+      </c>
+      <c r="F35" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G35" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -3653,7 +4162,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3669,34 +4178,34 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" t="s">
         <v>198</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>202</v>
-      </c>
       <c r="I1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J1" t="s">
+        <v>204</v>
+      </c>
+      <c r="K1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L1" t="s">
         <v>206</v>
-      </c>
-      <c r="K1" t="s">
-        <v>207</v>
-      </c>
-      <c r="L1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -3755,7 +4264,6 @@
         <v>16</v>
       </c>
       <c r="K3" t="e">
-        <f>IF(I3="","", VLOOKUP(I3, parent_children[[parent]:[children]], 2,'FALSE'))</f>
         <v>#NAME?</v>
       </c>
       <c r="L3" s="6" t="str">
@@ -3785,14 +4293,12 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="K4" t="str">
-        <f>IF(I4="","", VLOOKUP(I4, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
-      </c>
-      <c r="L4" s="6" t="b">
+      <c r="I4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6" t="e">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -3817,9 +4323,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="K5" t="str">
-        <f>IF(I5="","", VLOOKUP(I5, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K5" t="s">
+        <v>208</v>
       </c>
       <c r="L5" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -3848,9 +4353,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>29</v>
       </c>
-      <c r="K6" t="str">
-        <f>IF(I6="","", VLOOKUP(I6, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K6" t="s">
+        <v>208</v>
       </c>
       <c r="L6" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -3879,9 +4383,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="K7" t="str">
-        <f>IF(I7="","", VLOOKUP(I7, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K7" t="s">
+        <v>208</v>
       </c>
       <c r="L7" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -3896,7 +4399,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="6">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -3910,9 +4413,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>31</v>
       </c>
-      <c r="K8" t="str">
-        <f>IF(I8="","", VLOOKUP(I8, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K8" t="s">
+        <v>208</v>
       </c>
       <c r="L8" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -3927,7 +4429,7 @@
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -3941,9 +4443,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="K9" t="str">
-        <f>IF(I9="","", VLOOKUP(I9, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K9" t="s">
+        <v>208</v>
       </c>
       <c r="L9" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -3958,7 +4459,7 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E10">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -3972,9 +4473,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="K10" t="str">
-        <f>IF(I10="","", VLOOKUP(I10, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K10" t="s">
+        <v>208</v>
       </c>
       <c r="L10" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -3989,7 +4489,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4003,9 +4503,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="K11" t="str">
-        <f>IF(I11="","", VLOOKUP(I11, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K11" t="s">
+        <v>208</v>
       </c>
       <c r="L11" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4020,7 +4519,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E12">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4034,9 +4533,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="K12" t="str">
-        <f>IF(I12="","", VLOOKUP(I12, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K12" t="s">
+        <v>208</v>
       </c>
       <c r="L12" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4051,7 +4549,7 @@
         <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E13">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4065,9 +4563,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="K13" t="str">
-        <f>IF(I13="","", VLOOKUP(I13, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K13" t="s">
+        <v>208</v>
       </c>
       <c r="L13" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4082,7 +4579,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E14">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4096,9 +4593,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="K14" t="str">
-        <f>IF(I14="","", VLOOKUP(I14, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K14" t="s">
+        <v>208</v>
       </c>
       <c r="L14" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4113,7 +4609,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E15">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4127,9 +4623,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="K15" t="str">
-        <f>IF(I15="","", VLOOKUP(I15, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K15" t="s">
+        <v>208</v>
       </c>
       <c r="L15" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4144,7 +4639,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E16">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4158,9 +4653,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="K16" t="str">
-        <f>IF(I16="","", VLOOKUP(I16, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K16" t="s">
+        <v>208</v>
       </c>
       <c r="L16" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4175,7 +4669,7 @@
         <v>36</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E17">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4189,9 +4683,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="K17" t="str">
-        <f>IF(I17="","", VLOOKUP(I17, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K17" t="s">
+        <v>208</v>
       </c>
       <c r="L17" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4206,7 +4699,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E18">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4220,9 +4713,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="K18" t="str">
-        <f>IF(I18="","", VLOOKUP(I18, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K18" t="s">
+        <v>208</v>
       </c>
       <c r="L18" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4237,7 +4729,7 @@
         <v>36</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E19">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4251,9 +4743,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="K19" t="str">
-        <f>IF(I19="","", VLOOKUP(I19, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K19" t="s">
+        <v>208</v>
       </c>
       <c r="L19" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4268,7 +4759,7 @@
         <v>32</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4282,9 +4773,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="K20" t="str">
-        <f>IF(I20="","", VLOOKUP(I20, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K20" t="s">
+        <v>208</v>
       </c>
       <c r="L20" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4299,7 +4789,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4313,9 +4803,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="K21" t="str">
-        <f>IF(I21="","", VLOOKUP(I21, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K21" t="s">
+        <v>208</v>
       </c>
       <c r="L21" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4330,7 +4819,7 @@
         <v>32</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4344,9 +4833,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="K22" t="str">
-        <f>IF(I22="","", VLOOKUP(I22, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K22" t="s">
+        <v>208</v>
       </c>
       <c r="L22" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4361,7 +4849,7 @@
         <v>38</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E23">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4375,9 +4863,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>37</v>
       </c>
-      <c r="K23" t="str">
-        <f>IF(I23="","", VLOOKUP(I23, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K23" t="s">
+        <v>208</v>
       </c>
       <c r="L23" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4392,7 +4879,7 @@
         <v>38</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E24">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4406,9 +4893,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>38</v>
       </c>
-      <c r="K24" t="str">
-        <f>IF(I24="","", VLOOKUP(I24, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K24" t="s">
+        <v>208</v>
       </c>
       <c r="L24" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4423,7 +4909,7 @@
         <v>38</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E25">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
@@ -4437,9 +4923,8 @@
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>39</v>
       </c>
-      <c r="K25" t="str">
-        <f>IF(I25="","", VLOOKUP(I25, parent_children[[parent]:[children]], 2,'FALSE'))</f>
-        <v/>
+      <c r="K25" t="s">
+        <v>208</v>
       </c>
       <c r="L25" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
@@ -4468,8 +4953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4479,10 +4964,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21">
       <c r="A1" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4491,7 +4976,7 @@
         <v>Betonkerntemperierung</v>
       </c>
       <c r="B2" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A2,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A2,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>CCA</v>
       </c>
     </row>
@@ -4501,7 +4986,7 @@
         <v>Blockheizkraftwerk (BHKW)</v>
       </c>
       <c r="B3" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A3,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A3,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>CHP</v>
       </c>
     </row>
@@ -4511,7 +4996,7 @@
         <v>Fernkälte</v>
       </c>
       <c r="B4" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A4,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A4,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>C.DISCT</v>
       </c>
     </row>
@@ -4521,7 +5006,7 @@
         <v>Fernwärme</v>
       </c>
       <c r="B5" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A5,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A5,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>H.DISCT</v>
       </c>
     </row>
@@ -4531,7 +5016,7 @@
         <v>Freie Kühlung</v>
       </c>
       <c r="B6" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A6,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A6,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>C.FREE</v>
       </c>
     </row>
@@ -4541,7 +5026,7 @@
         <v>Gaskühler</v>
       </c>
       <c r="B7" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A7,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A7,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>C.GAS</v>
       </c>
     </row>
@@ -4551,7 +5036,7 @@
         <v>Gebäudeautomationssystem</v>
       </c>
       <c r="B8" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A8,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A8,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>BAS</v>
       </c>
     </row>
@@ -4561,7 +5046,7 @@
         <v>Gebäudemanagementsystem</v>
       </c>
       <c r="B9" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A9,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A9,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>BMS</v>
       </c>
     </row>
@@ -4571,7 +5056,7 @@
         <v>Kältemaschine</v>
       </c>
       <c r="B10" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A10,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A10,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>CH</v>
       </c>
     </row>
@@ -4581,7 +5066,7 @@
         <v>Kessel</v>
       </c>
       <c r="B11" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A11,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A11,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>BOI</v>
       </c>
     </row>
@@ -4591,7 +5076,7 @@
         <v>Kühlturm</v>
       </c>
       <c r="B12" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A12,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A12,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>C.TOW</v>
       </c>
     </row>
@@ -4601,7 +5086,7 @@
         <v>Luft</v>
       </c>
       <c r="B13" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A13,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A13,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>AIR</v>
       </c>
     </row>
@@ -4611,7 +5096,7 @@
         <v>Lüftungsmaschine</v>
       </c>
       <c r="B14" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A14,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A14,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>AHU</v>
       </c>
     </row>
@@ -4621,7 +5106,7 @@
         <v>Solarthermie</v>
       </c>
       <c r="B15" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A15,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A15,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>SOL.TH</v>
       </c>
     </row>
@@ -4631,7 +5116,7 @@
         <v>Speicher</v>
       </c>
       <c r="B16" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A16,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A16,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>STO</v>
       </c>
     </row>
@@ -4641,7 +5126,7 @@
         <v>Unterverteiler</v>
       </c>
       <c r="B17" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A17,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A17,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>DIST.SUB</v>
       </c>
     </row>
@@ -4651,7 +5136,7 @@
         <v>Unterverteilsystem</v>
       </c>
       <c r="B18" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A18,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A18,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>DISTS.SUB</v>
       </c>
     </row>
@@ -4661,7 +5146,7 @@
         <v>Verteiler</v>
       </c>
       <c r="B19" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A19,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A19,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>DIST</v>
       </c>
     </row>
@@ -4671,7 +5156,7 @@
         <v>Verteilsystem</v>
       </c>
       <c r="B20" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A20,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A20,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>DISTS</v>
       </c>
     </row>
@@ -4681,7 +5166,7 @@
         <v>Wärmepumpe</v>
       </c>
       <c r="B21" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A21,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A21,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>HP</v>
       </c>
     </row>
@@ -4691,107 +5176,121 @@
         <v>Wärmeübertrager</v>
       </c>
       <c r="B22" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A22,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A22,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v>HX</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="B23" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A23,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A23,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="B24" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A24,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A24,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="B25" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A25,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A25,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="B26" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A26,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A26,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="B27" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A27,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A27,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="B28" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A28,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A28,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="B29" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A29,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A29,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="B30" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A30,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A30,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="B31" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A31,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A31,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="B32" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A32,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A32,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A33,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A33,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A34,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A34,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A35,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A35,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A36,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A36,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A37,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A37,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A38,abbreviation[[description_german]:[abbreviation]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A38,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add changes SQL_table.xlsx (SQL commands)
</commit_message>
<xml_diff>
--- a/Excel-Table/SQL_table.xlsx
+++ b/Excel-Table/SQL_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="abbreviation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="216">
   <si>
     <t>Betonkerntemperierung</t>
   </si>
@@ -251,9 +251,6 @@
     <t>Verflüssiger</t>
   </si>
   <si>
-    <t>abbreviation</t>
-  </si>
-  <si>
     <t>category_id</t>
   </si>
   <si>
@@ -677,10 +674,13 @@
     <t>VARCHAR[30]</t>
   </si>
   <si>
-    <t>abbreviation_BUDO</t>
-  </si>
-  <si>
     <t>VARCHAR[200]</t>
+  </si>
+  <si>
+    <t>abbreviation_category_budo</t>
+  </si>
+  <si>
+    <t>abbreviation_budo</t>
   </si>
 </sst>
 </file>
@@ -788,6 +788,27 @@
   <dxfs count="18">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -855,27 +876,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -929,7 +929,7 @@
     <tableColumn id="1" name="abbreviation_id"/>
     <tableColumn id="2" name="description_german" dataDxfId="17"/>
     <tableColumn id="4" name="description_english" dataDxfId="16"/>
-    <tableColumn id="3" name="abbreviation_BUDO"/>
+    <tableColumn id="3" name="abbreviation_budo"/>
     <tableColumn id="5" name="abbreviation_id(for SVERWEIS)" dataDxfId="15">
       <calculatedColumnFormula>abbreviation[[#This Row],[abbreviation_id]]</calculatedColumnFormula>
     </tableColumn>
@@ -939,15 +939,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="category" displayName="category" ref="A2:F42" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="category" displayName="category" ref="A2:F42" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A2:F42"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="category_id" dataDxfId="5"/>
-    <tableColumn id="2" name="category_name_german" dataDxfId="4"/>
-    <tableColumn id="3" name="category_name_english" dataDxfId="3"/>
-    <tableColumn id="4" name="abbreviation" dataDxfId="2"/>
-    <tableColumn id="5" name="comment" dataDxfId="1"/>
-    <tableColumn id="6" name="category_id(for SVERWEIS)" dataDxfId="0">
+    <tableColumn id="1" name="category_id" dataDxfId="12"/>
+    <tableColumn id="2" name="category_name_german" dataDxfId="11"/>
+    <tableColumn id="3" name="category_name_english" dataDxfId="10"/>
+    <tableColumn id="4" name="abbreviation_category_budo" dataDxfId="9"/>
+    <tableColumn id="5" name="comment" dataDxfId="8"/>
+    <tableColumn id="6" name="category_id(for SVERWEIS)" dataDxfId="7">
       <calculatedColumnFormula>category[[#This Row],[category_id]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -956,8 +956,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="category_assignment" displayName="category_assignment" ref="A1:C49" totalsRowShown="0">
-  <autoFilter ref="A1:C49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="category_assignment" displayName="category_assignment" ref="A2:C50" totalsRowShown="0">
+  <autoFilter ref="A2:C50"/>
   <tableColumns count="3">
     <tableColumn id="1" name="category_assignment_id"/>
     <tableColumn id="2" name="category"/>
@@ -968,16 +968,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle8" displayName="Tabelle8" ref="E1:G35" totalsRowShown="0">
-  <autoFilter ref="E1:G35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle8" displayName="Tabelle8" ref="E2:G36" totalsRowShown="0">
+  <autoFilter ref="E2:G36"/>
   <tableColumns count="3">
     <tableColumn id="1" name="category_assignment_id">
       <calculatedColumnFormula>category_assignment[[#This Row],[category_assignment_id]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="category_id" dataDxfId="14">
+    <tableColumn id="2" name="category_id" dataDxfId="6">
       <calculatedColumnFormula>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="abbreviation_id" dataDxfId="13">
+    <tableColumn id="3" name="abbreviation_id" dataDxfId="5">
       <calculatedColumnFormula>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -986,8 +986,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="parent_children" displayName="parent_children" ref="A1:C25" totalsRowShown="0">
-  <autoFilter ref="A1:C25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="parent_children" displayName="parent_children" ref="A2:C26" totalsRowShown="0">
+  <autoFilter ref="A2:C26"/>
   <tableColumns count="3">
     <tableColumn id="1" name="parent_children_id"/>
     <tableColumn id="2" name="parent"/>
@@ -998,16 +998,16 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="parent_children8" displayName="parent_children8" ref="E1:G25" totalsRowShown="0">
-  <autoFilter ref="E1:G25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="parent_children8" displayName="parent_children8" ref="E2:G26" totalsRowShown="0">
+  <autoFilter ref="E2:G26"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="parent_children_id" dataDxfId="12">
+    <tableColumn id="1" name="parent_children_id" dataDxfId="4">
       <calculatedColumnFormula>parent_children[[#This Row],[parent_children_id]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="parent_id" dataDxfId="11">
+    <tableColumn id="2" name="parent_id" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="children_id" dataDxfId="10">
+    <tableColumn id="3" name="children_id" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1016,13 +1016,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="I1:L25" totalsRowShown="0">
-  <autoFilter ref="I1:L25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="I2:L26" totalsRowShown="0">
+  <autoFilter ref="I2:L26"/>
   <tableColumns count="4">
     <tableColumn id="1" name="System"/>
     <tableColumn id="2" name="."/>
-    <tableColumn id="3" name="System_2" dataDxfId="9"/>
-    <tableColumn id="4" name="System_3" dataDxfId="8">
+    <tableColumn id="3" name="System_2" dataDxfId="1"/>
+    <tableColumn id="4" name="System_3" dataDxfId="0">
       <calculatedColumnFormula>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1295,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1310,37 +1310,37 @@
   <sheetData>
     <row r="1" spans="1:7" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" t="s">
         <v>194</v>
       </c>
-      <c r="C2" t="s">
-        <v>195</v>
-      </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G2" t="str">
-        <f ca="1">"CREATE TABLE "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;"("&amp;abbreviation[[#Headers],[abbreviation_id]]&amp;" "&amp;A1&amp;","&amp;abbreviation[[#Headers],[description_german]]&amp;" "&amp;B1&amp;","&amp;abbreviation[[#Headers],[description_english]]&amp;" "&amp;C1&amp;","&amp;abbreviation[[#Headers],[abbreviation_BUDO]]&amp;" "&amp;D1&amp;", PRIMARY KEY("&amp;abbreviation[[#Headers],[abbreviation_id]]&amp;"))"</f>
-        <v>CREATE TABLE abbreviation(abbreviation_id INTEGER[10],description_german VARCHAR[1000],description_english VARCHAR[1000],abbreviation_BUDO VARCHAR[30], PRIMARY KEY(abbreviation_id))</v>
+        <f ca="1">"CREATE TABLE "&amp;RIGHT(CELL("dateiname",A1),LEN(CELL("dateiname",A1))-FIND("]",CELL("dateiname",A1)))&amp;"("&amp;abbreviation[[#Headers],[abbreviation_id]]&amp;" "&amp;A1&amp;","&amp;abbreviation[[#Headers],[description_german]]&amp;" "&amp;B1&amp;","&amp;abbreviation[[#Headers],[description_english]]&amp;" "&amp;C1&amp;","&amp;abbreviation[[#Headers],[abbreviation_budo]]&amp;" "&amp;D1&amp;", PRIMARY KEY("&amp;abbreviation[[#Headers],[abbreviation_id]]&amp;"))"</f>
+        <v>CREATE TABLE abbreviation(abbreviation_id INTEGER[10],description_german VARCHAR[1000],description_english VARCHAR[1000],abbreviation_budo VARCHAR[30], PRIMARY KEY(abbreviation_id))</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="6" customFormat="1">
@@ -1348,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3" s="3"/>
       <c r="E3" s="6">
@@ -1356,8 +1356,8 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (0,' ,,);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A1),LEN(CELL("dateiname",A1))-FIND("]",CELL("dateiname",A1)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (0,' ','','');</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1376,8 +1376,8 @@
         <v>1</v>
       </c>
       <c r="G4" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (1,Betonkerntemperierung,,CCA);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A2),LEN(CELL("dateiname",A2))-FIND("]",CELL("dateiname",A2)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (1,'Betonkerntemperierung','','CCA');</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1396,8 +1396,8 @@
         <v>2</v>
       </c>
       <c r="G5" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (2,Blockheizkraftwerk (BHKW),,CHP);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A3),LEN(CELL("dateiname",A3))-FIND("]",CELL("dateiname",A3)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (2,'Blockheizkraftwerk (BHKW)','','CHP');</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1416,8 +1416,8 @@
         <v>3</v>
       </c>
       <c r="G6" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (3,Fernkälte,,C.DISCT);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A4),LEN(CELL("dateiname",A4))-FIND("]",CELL("dateiname",A4)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (3,'Fernkälte','','C.DISCT');</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1436,8 +1436,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (4,Fernwärme,,H.DISCT);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A5),LEN(CELL("dateiname",A5))-FIND("]",CELL("dateiname",A5)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (4,'Fernwärme','','H.DISCT');</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1456,8 +1456,8 @@
         <v>5</v>
       </c>
       <c r="G8" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (5,Freie Kühlung,,C.FREE);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A6),LEN(CELL("dateiname",A6))-FIND("]",CELL("dateiname",A6)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (5,'Freie Kühlung','','C.FREE');</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1476,8 +1476,8 @@
         <v>6</v>
       </c>
       <c r="G9" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (6,Gaskühler,,C.GAS);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A7),LEN(CELL("dateiname",A7))-FIND("]",CELL("dateiname",A7)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (6,'Gaskühler','','C.GAS');</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1496,8 +1496,8 @@
         <v>7</v>
       </c>
       <c r="G10" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (7,Gebäudeautomationssystem,,BAS);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A8),LEN(CELL("dateiname",A8))-FIND("]",CELL("dateiname",A8)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (7,'Gebäudeautomationssystem','','BAS');</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1516,8 +1516,8 @@
         <v>8</v>
       </c>
       <c r="G11" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (8,Gebäudemanagementsystem,,BMS);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A9),LEN(CELL("dateiname",A9))-FIND("]",CELL("dateiname",A9)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (8,'Gebäudemanagementsystem','','BMS');</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1536,8 +1536,8 @@
         <v>9</v>
       </c>
       <c r="G12" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (9,Kältemaschine,,CH);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A10),LEN(CELL("dateiname",A10))-FIND("]",CELL("dateiname",A10)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (9,'Kältemaschine','','CH');</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1556,8 +1556,8 @@
         <v>10</v>
       </c>
       <c r="G13" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (10,Kessel,,BOI);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A11),LEN(CELL("dateiname",A11))-FIND("]",CELL("dateiname",A11)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (10,'Kessel','','BOI');</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1576,8 +1576,8 @@
         <v>11</v>
       </c>
       <c r="G14" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (11,Kühlturm,,C.TOW);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A12),LEN(CELL("dateiname",A12))-FIND("]",CELL("dateiname",A12)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (11,'Kühlturm','','C.TOW');</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1596,8 +1596,8 @@
         <v>12</v>
       </c>
       <c r="G15" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (12,Luft,,AIR);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A13),LEN(CELL("dateiname",A13))-FIND("]",CELL("dateiname",A13)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (12,'Luft','','AIR');</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1616,8 +1616,8 @@
         <v>13</v>
       </c>
       <c r="G16" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (13,Lüftungsmaschine,,AHU);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A14),LEN(CELL("dateiname",A14))-FIND("]",CELL("dateiname",A14)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (13,'Lüftungsmaschine','','AHU');</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1636,8 +1636,8 @@
         <v>14</v>
       </c>
       <c r="G17" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (14,Solarthermie,,SOL.TH);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A15),LEN(CELL("dateiname",A15))-FIND("]",CELL("dateiname",A15)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (14,'Solarthermie','','SOL.TH');</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1656,8 +1656,8 @@
         <v>15</v>
       </c>
       <c r="G18" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (15,Speicher,,STO);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A16),LEN(CELL("dateiname",A16))-FIND("]",CELL("dateiname",A16)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (15,'Speicher','','STO');</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1676,8 +1676,8 @@
         <v>16</v>
       </c>
       <c r="G19" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (16,Unterverteiler,,DIST.SUB);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A17),LEN(CELL("dateiname",A17))-FIND("]",CELL("dateiname",A17)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (16,'Unterverteiler','','DIST.SUB');</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1696,8 +1696,8 @@
         <v>17</v>
       </c>
       <c r="G20" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (17,Unterverteilsystem,,DISTS.SUB);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A18),LEN(CELL("dateiname",A18))-FIND("]",CELL("dateiname",A18)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (17,'Unterverteilsystem','','DISTS.SUB');</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1716,8 +1716,8 @@
         <v>18</v>
       </c>
       <c r="G21" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (18,Verteiler,,DIST);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A19),LEN(CELL("dateiname",A19))-FIND("]",CELL("dateiname",A19)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (18,'Verteiler','','DIST');</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1736,8 +1736,8 @@
         <v>19</v>
       </c>
       <c r="G22" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (19,Verteilsystem,,DISTS);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A20),LEN(CELL("dateiname",A20))-FIND("]",CELL("dateiname",A20)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (19,'Verteilsystem','','DISTS');</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1756,8 +1756,8 @@
         <v>20</v>
       </c>
       <c r="G23" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (20,Wärmepumpe,,HP);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A21),LEN(CELL("dateiname",A21))-FIND("]",CELL("dateiname",A21)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (20,'Wärmepumpe','','HP');</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1776,8 +1776,8 @@
         <v>21</v>
       </c>
       <c r="G24" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (21,Wärmeübertrager,,HX);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A22),LEN(CELL("dateiname",A22))-FIND("]",CELL("dateiname",A22)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (21,'Wärmeübertrager','','HX');</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1796,8 +1796,8 @@
         <v>22</v>
       </c>
       <c r="G25" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (22,Wasser,,WS);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A23),LEN(CELL("dateiname",A23))-FIND("]",CELL("dateiname",A23)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (22,'Wasser','','WS');</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1816,8 +1816,8 @@
         <v>23</v>
       </c>
       <c r="G26" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (23,Rückkühlung,,RCOO);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A24),LEN(CELL("dateiname",A24))-FIND("]",CELL("dateiname",A24)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (23,'Rückkühlung','','RCOO');</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1836,8 +1836,8 @@
         <v>24</v>
       </c>
       <c r="G27" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (24,Geothermiefeld,,GTF);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A25),LEN(CELL("dateiname",A25))-FIND("]",CELL("dateiname",A25)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (24,'Geothermiefeld','','GTF');</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1856,8 +1856,8 @@
         <v>25</v>
       </c>
       <c r="G28" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (25,Brennwertkessel,,COND);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A26),LEN(CELL("dateiname",A26))-FIND("]",CELL("dateiname",A26)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (25,'Brennwertkessel','','COND');</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1876,8 +1876,8 @@
         <v>26</v>
       </c>
       <c r="G29" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (26,Festbrennstoffkessel,,SFUEL);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A27),LEN(CELL("dateiname",A27))-FIND("]",CELL("dateiname",A27)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (26,'Festbrennstoffkessel','','SFUEL');</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1896,8 +1896,8 @@
         <v>27</v>
       </c>
       <c r="G30" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (27,Niedertemperaturkessel,,LT);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A28),LEN(CELL("dateiname",A28))-FIND("]",CELL("dateiname",A28)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (27,'Niedertemperaturkessel','','LT');</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1916,8 +1916,8 @@
         <v>28</v>
       </c>
       <c r="G31" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (28,Absorption,,ABSPT);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A29),LEN(CELL("dateiname",A29))-FIND("]",CELL("dateiname",A29)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (28,'Absorption','','ABSPT');</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1936,8 +1936,8 @@
         <v>29</v>
       </c>
       <c r="G32" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (29,Kompression,,COMP);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A30),LEN(CELL("dateiname",A30))-FIND("]",CELL("dateiname",A30)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (29,'Kompression','','COMP');</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1949,15 +1949,15 @@
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E33">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>30</v>
       </c>
       <c r="G33" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (30,Kältespeicher,,C.STO);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A31),LEN(CELL("dateiname",A31))-FIND("]",CELL("dateiname",A31)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (30,'Kältespeicher','','C.STO');</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1976,8 +1976,8 @@
         <v>31</v>
       </c>
       <c r="G34" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (31,Kombispeicher,,HDH);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A32),LEN(CELL("dateiname",A32))-FIND("]",CELL("dateiname",A32)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (31,'Kombispeicher','','HDH');</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1989,15 +1989,15 @@
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E35">
         <f>abbreviation[[#This Row],[abbreviation_id]]</f>
         <v>32</v>
       </c>
       <c r="G35" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (32,Wärmespeicher,,H.STO);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A33),LEN(CELL("dateiname",A33))-FIND("]",CELL("dateiname",A33)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (32,'Wärmespeicher','','H.STO');</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2016,8 +2016,8 @@
         <v>33</v>
       </c>
       <c r="G36" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (33,Warmwasser (TW),,DH);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A34),LEN(CELL("dateiname",A34))-FIND("]",CELL("dateiname",A34)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (33,'Warmwasser (TW)','','DH');</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2036,8 +2036,8 @@
         <v>34</v>
       </c>
       <c r="G37" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (34,Hochtemperatur,,HT);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A35),LEN(CELL("dateiname",A35))-FIND("]",CELL("dateiname",A35)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (34,'Hochtemperatur','','HT');</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2056,8 +2056,8 @@
         <v>35</v>
       </c>
       <c r="G38" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (35,Kälte,,CH);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A36),LEN(CELL("dateiname",A36))-FIND("]",CELL("dateiname",A36)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (35,'Kälte','','CH');</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2076,8 +2076,8 @@
         <v>36</v>
       </c>
       <c r="G39" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (36,Niedertemperatur,,LT);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A37),LEN(CELL("dateiname",A37))-FIND("]",CELL("dateiname",A37)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (36,'Niedertemperatur','','LT');</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2096,8 +2096,8 @@
         <v>37</v>
       </c>
       <c r="G40" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (37,Verdampfer,,EVAP);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A38),LEN(CELL("dateiname",A38))-FIND("]",CELL("dateiname",A38)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (37,'Verdampfer','','EVAP');</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2116,8 +2116,8 @@
         <v>38</v>
       </c>
       <c r="G41" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (38,Verdichter,,COMP);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A39),LEN(CELL("dateiname",A39))-FIND("]",CELL("dateiname",A39)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (38,'Verdichter','','COMP');</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2136,8 +2136,8 @@
         <v>39</v>
       </c>
       <c r="G42" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;","&amp;abbreviation[[#This Row],[description_german]]&amp;","&amp;abbreviation[[#This Row],[description_english]]&amp;","&amp;abbreviation[[#This Row],[abbreviation_BUDO]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (39,Verflüssiger,,COND);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A40),LEN(CELL("dateiname",A40))-FIND("]",CELL("dateiname",A40)))&amp;" VALUES"&amp;" ("&amp;abbreviation[[#This Row],[abbreviation_id]]&amp;",'"&amp;abbreviation[[#This Row],[description_german]]&amp;"','"&amp;abbreviation[[#This Row],[description_english]]&amp;"','"&amp;abbreviation[[#This Row],[abbreviation_budo]]&amp;"');"</f>
+        <v>INSERT INTO abbreviation VALUES (39,'Verflüssiger','','COND');</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2202,7 +2202,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="H3" sqref="H3:H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2210,50 +2210,50 @@
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="0.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>72</v>
+        <v>214</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="str">
-        <f ca="1">"CREATE TABLE "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;"("&amp;category[[#Headers],[category_id]]&amp;" "&amp;A1&amp;","&amp;category[[#Headers],[category_name_german]]&amp;" "&amp;B1&amp;","&amp;category[[#Headers],[category_name_english]]&amp;" "&amp;C1&amp;","&amp;category[[#Headers],[abbreviation]]&amp;" "&amp;D1&amp;","&amp;category[[#Headers],[comment]]&amp;" "&amp;E1&amp;", PRIMARY KEY("&amp;category[[#Headers],[category_id]]&amp;"))"</f>
-        <v>CREATE TABLE abbreviation(category_id INTEGER[10],category_name_german VARCHAR[200],category_name_english VARCHAR[200],abbreviation VARCHAR[30],comment VARCHAR[1000], PRIMARY KEY(category_id))</v>
+        <f ca="1">"CREATE TABLE "&amp;RIGHT(CELL("dateiname",A1),LEN(CELL("dateiname",A1))-FIND("]",CELL("dateiname",A1)))&amp;"("&amp;category[[#Headers],[category_id]]&amp;" "&amp;A1&amp;","&amp;category[[#Headers],[category_name_german]]&amp;" "&amp;B1&amp;","&amp;category[[#Headers],[category_name_english]]&amp;" "&amp;C1&amp;","&amp;category[[#Headers],[abbreviation_category_budo]]&amp;" "&amp;D1&amp;","&amp;category[[#Headers],[comment]]&amp;" "&amp;E1&amp;", PRIMARY KEY("&amp;category[[#Headers],[category_id]]&amp;"))"</f>
+        <v>CREATE TABLE category(category_id INTEGER[10],category_name_german VARCHAR[200],category_name_english VARCHAR[200],abbreviation_category_budo VARCHAR[30],comment VARCHAR[1000], PRIMARY KEY(category_id))</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1">
@@ -2269,8 +2269,8 @@
         <v>0</v>
       </c>
       <c r="H3" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;","&amp;category[[#This Row],[category_name_german]]&amp;","&amp;category[[#This Row],[category_name_english]]&amp;","&amp;category[[#This Row],[abbreviation]]&amp;","&amp;category[[#This Row],[comment]]&amp;");"</f>
-        <v>INSERT INTO abbreviation (0,,,,);</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A1),LEN(CELL("dateiname",A1))-FIND("]",CELL("dateiname",A1)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (0,'','','','');</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2278,24 +2278,24 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F4" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>1</v>
       </c>
       <c r="H4" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (1,'System','System','SYS','not used as abbrevation');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A2),LEN(CELL("dateiname",A2))-FIND("]",CELL("dateiname",A2)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (1,'System','System','SYS','not used as abbrevation');</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2303,24 +2303,24 @@
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F5" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>2</v>
       </c>
       <c r="H5" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (2,'Subsystem','Subsystem','SSYS','not used as abbrevation');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A3),LEN(CELL("dateiname",A3))-FIND("]",CELL("dateiname",A3)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (2,'Subsystem','Subsystem','SSYS','not used as abbrevation');</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2328,24 +2328,24 @@
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F6" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>3</v>
       </c>
       <c r="H6" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (3,'Subsubsystem','Subsubsystem','SSSYS','not used as abbrevation');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A4),LEN(CELL("dateiname",A4))-FIND("]",CELL("dateiname",A4)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (3,'Subsubsystem','Subsubsystem','SSSYS','not used as abbrevation');</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2353,24 +2353,24 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F7" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>4</v>
       </c>
       <c r="H7" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (4,'Medium','Medium','MED','not used as abbrevation');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A5),LEN(CELL("dateiname",A5))-FIND("]",CELL("dateiname",A5)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (4,'Medium','Medium','MED','not used as abbrevation');</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2378,24 +2378,24 @@
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F8" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>5</v>
       </c>
       <c r="H8" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (5,'Position Anlage','Position device','POSA','not used as abbrevation');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A6),LEN(CELL("dateiname",A6))-FIND("]",CELL("dateiname",A6)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (5,'Position Anlage','Position device','POSA','not used as abbrevation');</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2403,24 +2403,24 @@
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>189</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>190</v>
       </c>
       <c r="F9" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>6</v>
       </c>
       <c r="H9" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (6,'Datenpunkt','Data Point','DP','not used as abbrevation');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A7),LEN(CELL("dateiname",A7))-FIND("]",CELL("dateiname",A7)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (6,'Datenpunkt','Data Point','DP','not used as abbrevation');</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2428,24 +2428,24 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F10" s="7">
         <f>category[[#This Row],[category_id]]</f>
         <v>7</v>
       </c>
       <c r="H10" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (7,'Funktionsart','Function type','FT','not used as abbrevation');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A8),LEN(CELL("dateiname",A8))-FIND("]",CELL("dateiname",A8)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (7,'Funktionsart','Function type','FT','not used as abbrevation');</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2453,13 +2453,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7">
@@ -2467,8 +2467,8 @@
         <v>8</v>
       </c>
       <c r="H11" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (8,'Gebäude','building','BL','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A9),LEN(CELL("dateiname",A9))-FIND("]",CELL("dateiname",A9)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (8,'Gebäude','building','BL','');</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2476,13 +2476,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7">
@@ -2490,8 +2490,8 @@
         <v>9</v>
       </c>
       <c r="H12" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (9,'Liegenschaft/Standort/Werk','location','L','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A10),LEN(CELL("dateiname",A10))-FIND("]",CELL("dateiname",A10)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (9,'Liegenschaft/Standort/Werk','location','L','');</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2499,13 +2499,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7">
@@ -2513,8 +2513,8 @@
         <v>10</v>
       </c>
       <c r="H13" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (10,'Gewerk','craft','CR','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A11),LEN(CELL("dateiname",A11))-FIND("]",CELL("dateiname",A11)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (10,'Gewerk','craft','CR','');</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2522,13 +2522,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7">
@@ -2536,8 +2536,8 @@
         <v>11</v>
       </c>
       <c r="H14" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (11,'Raum Gerät','room device','R.D','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A12),LEN(CELL("dateiname",A12))-FIND("]",CELL("dateiname",A12)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (11,'Raum Gerät','room device','R.D','');</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2545,13 +2545,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
@@ -2559,8 +2559,8 @@
         <v>12</v>
       </c>
       <c r="H15" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (12,'Geschoss Gerät','floor device','FL.D','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A13),LEN(CELL("dateiname",A13))-FIND("]",CELL("dateiname",A13)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (12,'Geschoss Gerät','floor device','FL.D','');</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2568,13 +2568,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7">
@@ -2582,8 +2582,8 @@
         <v>13</v>
       </c>
       <c r="H16" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (13,'Gebäudeteil Gerät','section device','SC.D','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A14),LEN(CELL("dateiname",A14))-FIND("]",CELL("dateiname",A14)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (13,'Gebäudeteil Gerät','section device','SC.D','');</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2591,13 +2591,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7">
@@ -2605,8 +2605,8 @@
         <v>14</v>
       </c>
       <c r="H17" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (14,'Zone','zone','Z','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A15),LEN(CELL("dateiname",A15))-FIND("]",CELL("dateiname",A15)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (14,'Zone','zone','Z','');</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2614,13 +2614,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7">
@@ -2628,8 +2628,8 @@
         <v>15</v>
       </c>
       <c r="H18" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (15,'Fertigungsinsel/Fertigungslinie','production line','PL','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A16),LEN(CELL("dateiname",A16))-FIND("]",CELL("dateiname",A16)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (15,'Fertigungsinsel/Fertigungslinie','production line','PL','');</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2637,13 +2637,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7">
@@ -2651,8 +2651,8 @@
         <v>16</v>
       </c>
       <c r="H19" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (16,'Informationsschwerpunkt','information focus','ISP','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A17),LEN(CELL("dateiname",A17))-FIND("]",CELL("dateiname",A17)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (16,'Informationsschwerpunkt','information focus','ISP','');</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2660,13 +2660,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7">
@@ -2674,8 +2674,8 @@
         <v>17</v>
       </c>
       <c r="H20" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (17,'Wirtschaftseinheit/Kostengruppe','accounting entity','AE','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A18),LEN(CELL("dateiname",A18))-FIND("]",CELL("dateiname",A18)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (17,'Wirtschaftseinheit/Kostengruppe','accounting entity','AE','');</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2683,13 +2683,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7">
@@ -2697,8 +2697,8 @@
         <v>18</v>
       </c>
       <c r="H21" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (18,'Land','country','CTRY','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A19),LEN(CELL("dateiname",A19))-FIND("]",CELL("dateiname",A19)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (18,'Land','country','CTRY','');</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2706,13 +2706,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="8">
@@ -2720,8 +2720,8 @@
         <v>19</v>
       </c>
       <c r="H22" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (19,'Typ der Netzwerkanbindung','network protocol','NP','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A20),LEN(CELL("dateiname",A20))-FIND("]",CELL("dateiname",A20)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (19,'Typ der Netzwerkanbindung','network protocol','NP','');</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2729,13 +2729,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8">
@@ -2743,8 +2743,8 @@
         <v>20</v>
       </c>
       <c r="H23" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (20,'Netzwerknummer','network number','NET.N','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A21),LEN(CELL("dateiname",A21))-FIND("]",CELL("dateiname",A21)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (20,'Netzwerknummer','network number','NET.N','');</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2752,13 +2752,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8">
@@ -2766,8 +2766,8 @@
         <v>21</v>
       </c>
       <c r="H24" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (21,'Raum Schaltschrank','room control cabinet','R.CC','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A22),LEN(CELL("dateiname",A22))-FIND("]",CELL("dateiname",A22)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (21,'Raum Schaltschrank','room control cabinet','R.CC','');</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2775,13 +2775,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="8">
@@ -2789,8 +2789,8 @@
         <v>22</v>
       </c>
       <c r="H25" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (22,'Geschoss Schaltschrank','floor control cabinet','FL.CC','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A23),LEN(CELL("dateiname",A23))-FIND("]",CELL("dateiname",A23)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (22,'Geschoss Schaltschrank','floor control cabinet','FL.CC','');</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2798,13 +2798,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="8">
@@ -2812,8 +2812,8 @@
         <v>23</v>
       </c>
       <c r="H26" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (23,'Gebäudeteil Schaltschrank','section control cabinet','SC.CC','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A24),LEN(CELL("dateiname",A24))-FIND("]",CELL("dateiname",A24)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (23,'Gebäudeteil Schaltschrank','section control cabinet','SC.CC','');</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2821,13 +2821,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="8">
@@ -2835,8 +2835,8 @@
         <v>24</v>
       </c>
       <c r="H27" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (24,'Dokumentenart/Planart','document type','DT','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A25),LEN(CELL("dateiname",A25))-FIND("]",CELL("dateiname",A25)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (24,'Dokumentenart/Planart','document type','DT','');</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2844,13 +2844,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="8">
@@ -2858,8 +2858,8 @@
         <v>25</v>
       </c>
       <c r="H28" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (25,'Unternehmen','company','CMPY','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A26),LEN(CELL("dateiname",A26))-FIND("]",CELL("dateiname",A26)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (25,'Unternehmen','company','CMPY','');</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2867,13 +2867,13 @@
         <v>26</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8">
@@ -2881,8 +2881,8 @@
         <v>26</v>
       </c>
       <c r="H29" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (26,'Fabrikat/Hersteller','manufacturer','MAN','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A27),LEN(CELL("dateiname",A27))-FIND("]",CELL("dateiname",A27)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (26,'Fabrikat/Hersteller','manufacturer','MAN','');</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2890,13 +2890,13 @@
         <v>27</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="8">
@@ -2904,8 +2904,8 @@
         <v>27</v>
       </c>
       <c r="H30" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (27,'Servername','server name','SN','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A28),LEN(CELL("dateiname",A28))-FIND("]",CELL("dateiname",A28)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (27,'Servername','server name','SN','');</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2913,13 +2913,13 @@
         <v>28</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="8">
@@ -2927,8 +2927,8 @@
         <v>28</v>
       </c>
       <c r="H31" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (28,'Steuerungsgruppe','control group','CG','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A29),LEN(CELL("dateiname",A29))-FIND("]",CELL("dateiname",A29)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (28,'Steuerungsgruppe','control group','CG','');</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2936,13 +2936,13 @@
         <v>29</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>139</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="8">
@@ -2950,8 +2950,8 @@
         <v>29</v>
       </c>
       <c r="H32" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (29,'Größe','size','SZ','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A30),LEN(CELL("dateiname",A30))-FIND("]",CELL("dateiname",A30)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (29,'Größe','size','SZ','');</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2959,13 +2959,13 @@
         <v>30</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="8">
@@ -2973,8 +2973,8 @@
         <v>30</v>
       </c>
       <c r="H33" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (30,'Zählernummer','counter number','CN.N','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A31),LEN(CELL("dateiname",A31))-FIND("]",CELL("dateiname",A31)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (30,'Zählernummer','counter number','CN.N','');</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2982,13 +2982,13 @@
         <v>31</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="8">
@@ -2996,8 +2996,8 @@
         <v>31</v>
       </c>
       <c r="H34" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (31,'Achse','axis','AX','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A32),LEN(CELL("dateiname",A32))-FIND("]",CELL("dateiname",A32)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (31,'Achse','axis','AX','');</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -3005,13 +3005,13 @@
         <v>32</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="8">
@@ -3019,8 +3019,8 @@
         <v>32</v>
       </c>
       <c r="H35" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (32,'Straße','street','STR','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A33),LEN(CELL("dateiname",A33))-FIND("]",CELL("dateiname",A33)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (32,'Straße','street','STR','');</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -3028,13 +3028,13 @@
         <v>33</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>151</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8">
@@ -3042,8 +3042,8 @@
         <v>33</v>
       </c>
       <c r="H36" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (33,'Hausnummer','street number','STR.N','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A34),LEN(CELL("dateiname",A34))-FIND("]",CELL("dateiname",A34)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (33,'Hausnummer','street number','STR.N','');</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -3051,13 +3051,13 @@
         <v>34</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="8">
@@ -3065,8 +3065,8 @@
         <v>34</v>
       </c>
       <c r="H37" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (34,'Einheit','unit','U','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A35),LEN(CELL("dateiname",A35))-FIND("]",CELL("dateiname",A35)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (34,'Einheit','unit','U','');</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -3074,13 +3074,13 @@
         <v>35</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>157</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="8">
@@ -3088,8 +3088,8 @@
         <v>35</v>
       </c>
       <c r="H38" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (35,'Versorgter Raum','supplied room','R.SUP','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A36),LEN(CELL("dateiname",A36))-FIND("]",CELL("dateiname",A36)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (35,'Versorgter Raum','supplied room','R.SUP','');</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -3097,13 +3097,13 @@
         <v>36</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="D39" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="8">
@@ -3111,8 +3111,8 @@
         <v>36</v>
       </c>
       <c r="H39" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (36,'Versorgtes Geschoss','supplied floor','FL.SUP','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A37),LEN(CELL("dateiname",A37))-FIND("]",CELL("dateiname",A37)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (36,'Versorgtes Geschoss','supplied floor','FL.SUP','');</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -3120,13 +3120,13 @@
         <v>37</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="D40" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="8">
@@ -3134,8 +3134,8 @@
         <v>37</v>
       </c>
       <c r="H40" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (37,'Versorgte Zone','supplied zone','Z.SUP','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A38),LEN(CELL("dateiname",A38))-FIND("]",CELL("dateiname",A38)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (37,'Versorgte Zone','supplied zone','Z.SUP','');</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -3143,13 +3143,13 @@
         <v>38</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="D41" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="8">
@@ -3157,8 +3157,8 @@
         <v>38</v>
       </c>
       <c r="H41" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (38,'Versorgter Gebäudeteil','supplied section','SC.SUP','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A39),LEN(CELL("dateiname",A39))-FIND("]",CELL("dateiname",A39)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (38,'Versorgter Gebäudeteil','supplied section','SC.SUP','');</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -3166,13 +3166,13 @@
         <v>39</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="D42" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>169</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="8">
@@ -3180,8 +3180,8 @@
         <v>39</v>
       </c>
       <c r="H42" s="6" t="str">
-        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname"),LEN(CELL("dateiname"))-FIND("]",CELL("dateiname")))&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
-        <v>INSERT INTO abbreviation (39,'Versorgtes Gebäude','supplied building','BL.SUP','');</v>
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A40),LEN(CELL("dateiname",A40))-FIND("]",CELL("dateiname",A40)))&amp;" VALUES"&amp;" ("&amp;category[[#This Row],[category_id]]&amp;",'"&amp;category[[#This Row],[category_name_german]]&amp;"','"&amp;category[[#This Row],[category_name_english]]&amp;"','"&amp;category[[#This Row],[abbreviation_category_budo]]&amp;"','"&amp;category[[#This Row],[comment]]&amp;"');"</f>
+        <v>INSERT INTO category VALUES (39,'Versorgtes Gebäude','supplied building','BL.SUP','');</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -3249,10 +3249,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="A6:G9"/>
+      <selection activeCell="I3" sqref="I3:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3267,62 +3267,54 @@
     <col min="10" max="10" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1">
+      <c r="E1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="6" t="str">
+        <f ca="1">"CREATE TABLE "&amp;RIGHT(CELL("dateiname",A1),LEN(CELL("dateiname",A1))-FIND("]",CELL("dateiname",A1)))&amp;"("&amp;Tabelle8[[#Headers],[category_assignment_id]]&amp;" "&amp;E1&amp;","&amp;Tabelle8[[#Headers],[category_id]]&amp;" "&amp;F1&amp;","&amp;Tabelle8[[#Headers],[abbreviation_id]]&amp;" "&amp;G1&amp;", PRIMARY KEY("&amp;Tabelle8[[#Headers],[category_assignment_id]]&amp;"))"</f>
+        <v>CREATE TABLE category_assignment(category_assignment_id INTEGER[10],category_id INTEGER[10],abbreviation_id INTEGER[10], PRIMARY KEY(category_assignment_id))</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
         <v>191</v>
       </c>
-      <c r="B1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
         <v>1</v>
-      </c>
-      <c r="F2">
-        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6">
-        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>2</v>
       </c>
       <c r="F3">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3330,23 +3322,26 @@
       </c>
       <c r="G3">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A1),LEN(CELL("dateiname",A1))-FIND("]",CELL("dateiname",A1)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (1,1,1);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
       <c r="B4" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3354,23 +3349,26 @@
       </c>
       <c r="G4">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="I4" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="I4" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A2),LEN(CELL("dateiname",A2))-FIND("]",CELL("dateiname",A2)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (2,1,2);</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="E5" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3378,23 +3376,26 @@
       </c>
       <c r="G5">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="I5" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="I5" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A3),LEN(CELL("dateiname",A3))-FIND("]",CELL("dateiname",A3)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (3,1,3);</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E6" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3402,23 +3403,26 @@
       </c>
       <c r="G6">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="I6" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="I6" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A4),LEN(CELL("dateiname",A4))-FIND("]",CELL("dateiname",A4)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (4,1,4);</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3426,23 +3430,26 @@
       </c>
       <c r="G7">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>6</v>
-      </c>
-      <c r="I7" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="I7" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A5),LEN(CELL("dateiname",A5))-FIND("]",CELL("dateiname",A5)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (5,1,5);</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3450,23 +3457,26 @@
       </c>
       <c r="G8">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="I8" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="I8" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A6),LEN(CELL("dateiname",A6))-FIND("]",CELL("dateiname",A6)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (6,1,6);</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3474,23 +3484,26 @@
       </c>
       <c r="G9">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>8</v>
-      </c>
-      <c r="I9" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="I9" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A7),LEN(CELL("dateiname",A7))-FIND("]",CELL("dateiname",A7)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (7,1,7);</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3498,23 +3511,26 @@
       </c>
       <c r="G10">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>9</v>
-      </c>
-      <c r="I10" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="I10" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A8),LEN(CELL("dateiname",A8))-FIND("]",CELL("dateiname",A8)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (8,1,8);</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3522,23 +3538,26 @@
       </c>
       <c r="G11">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>10</v>
-      </c>
-      <c r="I11" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="I11" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A9),LEN(CELL("dateiname",A9))-FIND("]",CELL("dateiname",A9)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (9,1,9);</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3546,23 +3565,26 @@
       </c>
       <c r="G12">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>11</v>
-      </c>
-      <c r="I12" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="I12" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A10),LEN(CELL("dateiname",A10))-FIND("]",CELL("dateiname",A10)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (10,1,10);</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3570,23 +3592,26 @@
       </c>
       <c r="G13">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>12</v>
-      </c>
-      <c r="I13" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="I13" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A11),LEN(CELL("dateiname",A11))-FIND("]",CELL("dateiname",A11)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (11,1,11);</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3594,23 +3619,26 @@
       </c>
       <c r="G14">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>13</v>
-      </c>
-      <c r="I14" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A12),LEN(CELL("dateiname",A12))-FIND("]",CELL("dateiname",A12)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (12,1,12);</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3618,23 +3646,26 @@
       </c>
       <c r="G15">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>14</v>
-      </c>
-      <c r="I15" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="I15" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A13),LEN(CELL("dateiname",A13))-FIND("]",CELL("dateiname",A13)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (13,1,13);</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3642,23 +3673,26 @@
       </c>
       <c r="G16">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>15</v>
-      </c>
-      <c r="I16" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="I16" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A14),LEN(CELL("dateiname",A14))-FIND("]",CELL("dateiname",A14)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (14,1,14);</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E17" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3666,23 +3700,26 @@
       </c>
       <c r="G17">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="I17" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="I17" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A15),LEN(CELL("dateiname",A15))-FIND("]",CELL("dateiname",A15)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (15,1,15);</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3690,23 +3727,26 @@
       </c>
       <c r="G18">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>17</v>
-      </c>
-      <c r="I18" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="I18" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A16),LEN(CELL("dateiname",A16))-FIND("]",CELL("dateiname",A16)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (16,1,16);</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3714,23 +3754,26 @@
       </c>
       <c r="G19">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>18</v>
-      </c>
-      <c r="I19" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="I19" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A17),LEN(CELL("dateiname",A17))-FIND("]",CELL("dateiname",A17)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (17,1,17);</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3738,23 +3781,26 @@
       </c>
       <c r="G20">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>19</v>
-      </c>
-      <c r="I20" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="I20" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A18),LEN(CELL("dateiname",A18))-FIND("]",CELL("dateiname",A18)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (18,1,18);</v>
+      </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="6">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E21" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3762,23 +3808,26 @@
       </c>
       <c r="G21">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>20</v>
-      </c>
-      <c r="I21" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="I21" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A19),LEN(CELL("dateiname",A19))-FIND("]",CELL("dateiname",A19)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (19,1,19);</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E22" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F22">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3786,23 +3835,26 @@
       </c>
       <c r="G22">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>21</v>
-      </c>
-      <c r="I22" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="I22" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A20),LEN(CELL("dateiname",A20))-FIND("]",CELL("dateiname",A20)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (20,1,20);</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3810,23 +3862,26 @@
       </c>
       <c r="G23">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>22</v>
-      </c>
-      <c r="I23" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="I23" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A21),LEN(CELL("dateiname",A21))-FIND("]",CELL("dateiname",A21)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (21,1,21);</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E24" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3834,23 +3889,26 @@
       </c>
       <c r="G24">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="I24" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A22),LEN(CELL("dateiname",A22))-FIND("]",CELL("dateiname",A22)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (22,1,22);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="6">
         <v>23</v>
       </c>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25">
-        <v>24</v>
-      </c>
       <c r="B25" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" s="6">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3858,65 +3916,74 @@
       </c>
       <c r="G25">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="I25" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A23),LEN(CELL("dateiname",A23))-FIND("]",CELL("dateiname",A23)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (23,1,23);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="6">
+      <c r="B26" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="6">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>24</v>
+      </c>
+      <c r="F26">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="I26" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A24),LEN(CELL("dateiname",A24))-FIND("]",CELL("dateiname",A24)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (24,1,24);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="6">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>172</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B27" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" t="s">
         <v>2</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
         <v>25</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F27" s="11">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G27" s="11">
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="I26" s="6" t="str">
-        <f t="array" ref="I26">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I25))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="6">
+      <c r="I27" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A25),LEN(CELL("dateiname",A25))-FIND("]",CELL("dateiname",A25)))&amp;" VALUES"&amp;" ("&amp;Tabelle8[[#This Row],[category_assignment_id]]&amp;","&amp;Tabelle8[[#This Row],[category_id]]&amp;","&amp;Tabelle8[[#This Row],[abbreviation_id]]&amp;");"</f>
+        <v>INSERT INTO category_assignment VALUES (25,2,2);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="6">
         <v>26</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
         <v>26</v>
-      </c>
-      <c r="F27" s="11" t="e">
-        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G27" s="11" t="e">
-        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I27" s="6" t="str">
-        <f t="array" ref="I27">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I26))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="6">
-        <v>27</v>
-      </c>
-      <c r="E28">
-        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>27</v>
       </c>
       <c r="F28" s="11" t="e">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3927,17 +3994,17 @@
         <v>#N/A</v>
       </c>
       <c r="I28" s="6" t="str">
-        <f t="array" ref="I28">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I27))),"")</f>
+        <f t="array" ref="I28">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$2)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$2)+1-ROW(I27))),"")</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="6">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E29">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F29" s="11" t="e">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3948,17 +4015,17 @@
         <v>#N/A</v>
       </c>
       <c r="I29" s="6" t="str">
-        <f t="array" ref="I29">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I28))),"")</f>
+        <f t="array" ref="I29">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$2)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$2)+1-ROW(I28))),"")</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="6">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F30" s="11" t="e">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3969,17 +4036,17 @@
         <v>#N/A</v>
       </c>
       <c r="I30" s="6" t="str">
-        <f t="array" ref="I30">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I29))),"")</f>
+        <f t="array" ref="I30">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$2)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$2)+1-ROW(I29))),"")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E31">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F31" s="11" t="e">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -3990,17 +4057,17 @@
         <v>#N/A</v>
       </c>
       <c r="I31" s="6" t="str">
-        <f t="array" ref="I31">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I30))),"")</f>
+        <f t="array" ref="I31">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$2)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$2)+1-ROW(I30))),"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="6">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F32" s="11" t="e">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -4011,17 +4078,17 @@
         <v>#N/A</v>
       </c>
       <c r="I32" s="6" t="str">
-        <f t="array" ref="I32">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I31))),"")</f>
+        <f t="array" ref="I32">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$2)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$2)+1-ROW(I31))),"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="6">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E33">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F33" s="11" t="e">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -4032,17 +4099,17 @@
         <v>#N/A</v>
       </c>
       <c r="I33" s="6" t="str">
-        <f t="array" ref="I33">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$1)+1-ROW(I32))),"")</f>
+        <f t="array" ref="I33">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$2)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$2)+1-ROW(I32))),"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="6">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E34">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F34" s="11" t="e">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -4052,14 +4119,18 @@
         <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>#N/A</v>
       </c>
+      <c r="I34" s="6" t="str">
+        <f t="array" ref="I34">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$I$2)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$I$2)+1-ROW(I33))),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="6">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35">
         <f>category_assignment[[#This Row],[category_assignment_id]]</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F35" s="11" t="e">
         <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
@@ -4072,80 +4143,97 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="6">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E36">
+        <f>category_assignment[[#This Row],[category_assignment_id]]</f>
+        <v>34</v>
+      </c>
+      <c r="F36" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[category]],category[[category_name_german]:[category_id(for SVERWEIS)]],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G36" s="11" t="e">
+        <f>VLOOKUP(category_assignment[[#This Row],[description_german]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="6">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="6">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="6">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="6">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="6">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="6">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="6">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="6">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="6">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="6">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="6">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B50">
       <formula1>category_name_german</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C50">
       <formula1>description_german</formula1>
     </dataValidation>
   </dataValidations>
@@ -4159,10 +4247,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4170,87 +4258,75 @@
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="12" width="0" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" s="6" customFormat="1">
+      <c r="E1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
         <v>196</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>197</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="I1" t="s">
-        <v>171</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="I2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" t="s">
+        <v>203</v>
+      </c>
+      <c r="K2" t="s">
         <v>204</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L2" t="s">
         <v>205</v>
       </c>
-      <c r="L1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2">
+      <c r="N2" s="6" t="str">
+        <f ca="1">"CREATE TABLE "&amp;RIGHT(CELL("dateiname",A1),LEN(CELL("dateiname",A1))-FIND("]",CELL("dateiname",A1)))&amp;"("&amp;parent_children8[[#Headers],[parent_children_id]]&amp;" "&amp;E1&amp;","&amp;parent_children8[[#Headers],[parent_id]]&amp;" "&amp;F1&amp;","&amp;parent_children8[[#Headers],[children_id]]&amp;" "&amp;G1&amp;", PRIMARY KEY("&amp;parent_children8[[#Headers],[parent_children_id]]&amp;"))"</f>
+        <v>CREATE TABLE parent_children(parent_children_id INTEGER[10],parent_id INTEGER[10],children_id INTEGER[10], PRIMARY KEY(parent_children_id))</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E3" s="6">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
         <v>1</v>
-      </c>
-      <c r="F2" s="6">
-        <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>10</v>
-      </c>
-      <c r="G2" s="6">
-        <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="str">
-        <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
-        <v>Brennwertkessel</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="6">
-        <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>2</v>
       </c>
       <c r="F3" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4258,32 +4334,33 @@
       </c>
       <c r="G3" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>26</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="L3" s="6" t="str">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="str">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
-        <v>Absorption</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>Brennwertkessel</v>
+      </c>
+      <c r="N3" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A1),LEN(CELL("dateiname",A1))-FIND("]",CELL("dateiname",A1)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (1,10,25);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="6">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4291,59 +4368,70 @@
       </c>
       <c r="G4" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L4" s="6" t="str">
+        <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
+        <v>Absorption</v>
+      </c>
+      <c r="N4" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A2),LEN(CELL("dateiname",A2))-FIND("]",CELL("dateiname",A2)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (2,10,26);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="6">
+        <f>parent_children[[#This Row],[parent_children_id]]</f>
+        <v>3</v>
+      </c>
+      <c r="F5" s="6">
+        <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="G5" s="6">
+        <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="6" t="e">
+      <c r="L5" s="6" t="e">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5">
+      <c r="N5" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A3),LEN(CELL("dateiname",A3))-FIND("]",CELL("dateiname",A3)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (3,10,27);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E6" s="6">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
         <v>4</v>
-      </c>
-      <c r="F5" s="6">
-        <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>9</v>
-      </c>
-      <c r="G5" s="6">
-        <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>28</v>
-      </c>
-      <c r="K5" t="s">
-        <v>208</v>
-      </c>
-      <c r="L5" s="6" t="b">
-        <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="6">
-        <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>5</v>
       </c>
       <c r="F6" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4351,59 +4439,67 @@
       </c>
       <c r="G6" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L6" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="N6" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A4),LEN(CELL("dateiname",A4))-FIND("]",CELL("dateiname",A4)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (4,9,28);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" s="6">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G7" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L7" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="N7" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A5),LEN(CELL("dateiname",A5))-FIND("]",CELL("dateiname",A5)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (5,9,29);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="6">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4411,29 +4507,33 @@
       </c>
       <c r="G8" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L8" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="6">
-        <v>8</v>
+      <c r="N8" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A6),LEN(CELL("dateiname",A6))-FIND("]",CELL("dateiname",A6)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (6,15,30);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9">
+      <c r="C9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="6">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4441,29 +4541,33 @@
       </c>
       <c r="G9" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L9" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="N9" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A7),LEN(CELL("dateiname",A7))-FIND("]",CELL("dateiname",A7)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (7,15,31);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4471,59 +4575,67 @@
       </c>
       <c r="G10" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L10" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="N10" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A8),LEN(CELL("dateiname",A8))-FIND("]",CELL("dateiname",A8)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (8,15,32);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
       </c>
       <c r="E11">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G11" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L11" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="N11" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A9),LEN(CELL("dateiname",A9))-FIND("]",CELL("dateiname",A9)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (9,15,33);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4531,29 +4643,33 @@
       </c>
       <c r="G12" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L12" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="N12" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A10),LEN(CELL("dateiname",A10))-FIND("]",CELL("dateiname",A10)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (10,18,34);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4561,59 +4677,67 @@
       </c>
       <c r="G13" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L13" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="N13" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A11),LEN(CELL("dateiname",A11))-FIND("]",CELL("dateiname",A11)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (11,18,35);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="6">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E14">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G14" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L14" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="N14" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A12),LEN(CELL("dateiname",A12))-FIND("]",CELL("dateiname",A12)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (12,18,36);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="6">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E15">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4621,29 +4745,33 @@
       </c>
       <c r="G15" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L15" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="N15" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A13),LEN(CELL("dateiname",A13))-FIND("]",CELL("dateiname",A13)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (13,16,34);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4651,59 +4779,67 @@
       </c>
       <c r="G16" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L16" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="N16" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A14),LEN(CELL("dateiname",A14))-FIND("]",CELL("dateiname",A14)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (14,16,35);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="6">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E17">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G17" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L17" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="N17" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A15),LEN(CELL("dateiname",A15))-FIND("]",CELL("dateiname",A15)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (15,16,36);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="6">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E18">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4711,29 +4847,33 @@
       </c>
       <c r="G18" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L18" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="N18" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A16),LEN(CELL("dateiname",A16))-FIND("]",CELL("dateiname",A16)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (16,19,34);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4741,59 +4881,67 @@
       </c>
       <c r="G19" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L19" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="N19" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A17),LEN(CELL("dateiname",A17))-FIND("]",CELL("dateiname",A17)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (17,19,35);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E20">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G20" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L20" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="N20" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A18),LEN(CELL("dateiname",A18))-FIND("]",CELL("dateiname",A18)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (18,19,36);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="6">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E21">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4801,29 +4949,33 @@
       </c>
       <c r="G21" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L21" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="N21" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A19),LEN(CELL("dateiname",A19))-FIND("]",CELL("dateiname",A19)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (19,17,34);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F22" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4831,59 +4983,67 @@
       </c>
       <c r="G22" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L22" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="N22" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A20),LEN(CELL("dateiname",A20))-FIND("]",CELL("dateiname",A20)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (20,17,35);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E23">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G23" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L23" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="N23" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A21),LEN(CELL("dateiname",A21))-FIND("]",CELL("dateiname",A21)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (21,17,36);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E24">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4891,29 +5051,33 @@
       </c>
       <c r="G24" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L24" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="N24" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A22),LEN(CELL("dateiname",A22))-FIND("]",CELL("dateiname",A22)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (22,20,37);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E25">
         <f>parent_children[[#This Row],[parent_children_id]]</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
@@ -4921,22 +5085,60 @@
       </c>
       <c r="G25" s="6">
         <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L25" s="6" t="b">
         <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="6"/>
+      <c r="N25" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A23),LEN(CELL("dateiname",A23))-FIND("]",CELL("dateiname",A23)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (23,20,38);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="6">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26">
+        <f>parent_children[[#This Row],[parent_children_id]]</f>
+        <v>24</v>
+      </c>
+      <c r="F26" s="6">
+        <f>VLOOKUP(parent_children[[#This Row],[parent]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="G26" s="6">
+        <f>VLOOKUP(parent_children[[#This Row],[children]],abbreviation[[description_german]:[abbreviation_id(for SVERWEIS)]],4,FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="K26" t="s">
+        <v>207</v>
+      </c>
+      <c r="L26" s="6" t="b">
+        <f>IF(Tabelle2[[#This Row],[System]]&lt;&gt;"",VLOOKUP(Tabelle2[[#This Row],[System]],parent_children[[parent]:[children]],2,0))</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="6" t="str">
+        <f ca="1">"INSERT INTO "&amp;RIGHT(CELL("dateiname",A24),LEN(CELL("dateiname",A24))-FIND("]",CELL("dateiname",A24)))&amp;" VALUES"&amp;" ("&amp;parent_children8[[#This Row],[parent_children_id]]&amp;","&amp;parent_children8[[#This Row],[parent_id]]&amp;","&amp;parent_children8[[#This Row],[children_id]]&amp;");"</f>
+        <v>INSERT INTO parent_children VALUES (24,20,39);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C25 I2:I4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:C26 I3:I5">
       <formula1>description_german</formula1>
     </dataValidation>
   </dataValidations>
@@ -4964,315 +5166,315 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21">
       <c r="A1" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="str">
         <f t="array" ref="A2">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A1))),"")</f>
-        <v>Betonkerntemperierung</v>
+        <v>Blockheizkraftwerk (BHKW)</v>
       </c>
       <c r="B2" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A2,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>CCA</v>
+        <f>IFERROR(VLOOKUP(A2,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>CHP</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="6" t="str">
         <f t="array" ref="A3">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A2))),"")</f>
-        <v>Blockheizkraftwerk (BHKW)</v>
+        <v>Fernkälte</v>
       </c>
       <c r="B3" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A3,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>CHP</v>
+        <f>IFERROR(VLOOKUP(A3,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>C.DISCT</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="6" t="str">
         <f t="array" ref="A4">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A3))),"")</f>
-        <v>Fernkälte</v>
+        <v>Fernwärme</v>
       </c>
       <c r="B4" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A4,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>C.DISCT</v>
+        <f>IFERROR(VLOOKUP(A4,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>H.DISCT</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="str">
         <f t="array" ref="A5">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A4))),"")</f>
-        <v>Fernwärme</v>
+        <v>Freie Kühlung</v>
       </c>
       <c r="B5" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A5,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>H.DISCT</v>
+        <f>IFERROR(VLOOKUP(A5,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>C.FREE</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="6" t="str">
         <f t="array" ref="A6">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A5))),"")</f>
-        <v>Freie Kühlung</v>
+        <v>Gaskühler</v>
       </c>
       <c r="B6" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A6,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>C.FREE</v>
+        <f>IFERROR(VLOOKUP(A6,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>C.GAS</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="6" t="str">
         <f t="array" ref="A7">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A6))),"")</f>
-        <v>Gaskühler</v>
+        <v>Gebäudeautomationssystem</v>
       </c>
       <c r="B7" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A7,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>C.GAS</v>
+        <f>IFERROR(VLOOKUP(A7,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>BAS</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="str">
         <f t="array" ref="A8">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A7))),"")</f>
-        <v>Gebäudeautomationssystem</v>
+        <v>Gebäudemanagementsystem</v>
       </c>
       <c r="B8" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A8,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>BAS</v>
+        <f>IFERROR(VLOOKUP(A8,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>BMS</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="6" t="str">
         <f t="array" ref="A9">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A8))),"")</f>
-        <v>Gebäudemanagementsystem</v>
+        <v>Kältemaschine</v>
       </c>
       <c r="B9" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A9,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>BMS</v>
+        <f>IFERROR(VLOOKUP(A9,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>CH</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="6" t="str">
         <f t="array" ref="A10">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A9))),"")</f>
-        <v>Kältemaschine</v>
+        <v>Kessel</v>
       </c>
       <c r="B10" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A10,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>CH</v>
+        <f>IFERROR(VLOOKUP(A10,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>BOI</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="6" t="str">
         <f t="array" ref="A11">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A10))),"")</f>
-        <v>Kessel</v>
+        <v>Kühlturm</v>
       </c>
       <c r="B11" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A11,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>BOI</v>
+        <f>IFERROR(VLOOKUP(A11,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>C.TOW</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6" t="str">
         <f t="array" ref="A12">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A11))),"")</f>
-        <v>Kühlturm</v>
+        <v>Luft</v>
       </c>
       <c r="B12" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A12,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>C.TOW</v>
+        <f>IFERROR(VLOOKUP(A12,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>AIR</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="6" t="str">
         <f t="array" ref="A13">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A12))),"")</f>
-        <v>Luft</v>
+        <v>Lüftungsmaschine</v>
       </c>
       <c r="B13" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A13,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>AIR</v>
+        <f>IFERROR(VLOOKUP(A13,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>AHU</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="6" t="str">
         <f t="array" ref="A14">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A13))),"")</f>
-        <v>Lüftungsmaschine</v>
+        <v>Solarthermie</v>
       </c>
       <c r="B14" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A14,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>AHU</v>
+        <f>IFERROR(VLOOKUP(A14,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>SOL.TH</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="6" t="str">
         <f t="array" ref="A15">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A14))),"")</f>
-        <v>Solarthermie</v>
+        <v>Speicher</v>
       </c>
       <c r="B15" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A15,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>SOL.TH</v>
+        <f>IFERROR(VLOOKUP(A15,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>STO</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="6" t="str">
         <f t="array" ref="A16">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A15))),"")</f>
-        <v>Speicher</v>
+        <v>Unterverteiler</v>
       </c>
       <c r="B16" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A16,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>STO</v>
+        <f>IFERROR(VLOOKUP(A16,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>DIST.SUB</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="6" t="str">
         <f t="array" ref="A17">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A16))),"")</f>
-        <v>Unterverteiler</v>
+        <v>Unterverteilsystem</v>
       </c>
       <c r="B17" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A17,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>DIST.SUB</v>
+        <f>IFERROR(VLOOKUP(A17,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>DISTS.SUB</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="6" t="str">
         <f t="array" ref="A18">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A17))),"")</f>
-        <v>Unterverteilsystem</v>
+        <v>Verteiler</v>
       </c>
       <c r="B18" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A18,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>DISTS.SUB</v>
+        <f>IFERROR(VLOOKUP(A18,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>DIST</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="6" t="str">
         <f t="array" ref="A19">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A18))),"")</f>
-        <v>Verteiler</v>
+        <v>Verteilsystem</v>
       </c>
       <c r="B19" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A19,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>DIST</v>
+        <f>IFERROR(VLOOKUP(A19,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>DISTS</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="6" t="str">
         <f t="array" ref="A20">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A19))),"")</f>
-        <v>Verteilsystem</v>
+        <v>Wärmepumpe</v>
       </c>
       <c r="B20" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A20,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>DISTS</v>
+        <f>IFERROR(VLOOKUP(A20,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>HP</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="6" t="str">
         <f t="array" ref="A21">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A20))),"")</f>
-        <v>Wärmepumpe</v>
+        <v>Wärmeübertrager</v>
       </c>
       <c r="B21" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A21,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>HP</v>
+        <f>IFERROR(VLOOKUP(A21,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>HX</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="6" t="str">
         <f t="array" ref="A22">IFERROR(INDEX(category_assignment[description_german],LARGE((category_assignment[category]=$A$1)*(ROW(category_assignment[category])-2),COUNTIF(category_assignment[category],$A$1)-ROW(A21))),"")</f>
-        <v>Wärmeübertrager</v>
+        <v>Wasser</v>
       </c>
       <c r="B22" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A22,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
-        <v>HX</v>
+        <f>IFERROR(VLOOKUP(A22,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
+        <v>WS</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="B23" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A23,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A23,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="B24" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A24,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A24,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="B25" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A25,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A25,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="B26" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A26,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A26,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="B27" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A27,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A27,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="B28" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A28,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A28,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="B29" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A29,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A29,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="B30" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A30,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A30,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="B31" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A31,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A31,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="B32" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A32,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A32,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A33,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A33,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A34,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A34,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A35,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A35,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A36,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A36,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A37,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A37,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="6" t="str">
-        <f>IFERROR(VLOOKUP(A38,abbreviation[[description_german]:[abbreviation_BUDO]],3,0),"")</f>
+        <f>IFERROR(VLOOKUP(A38,abbreviation[[description_german]:[abbreviation_budo]],3,0),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>